<commit_message>
Updated tfidf csvs and Glove SVM results
</commit_message>
<xml_diff>
--- a/TREC/50_Results/Progress Summary.xlsx
+++ b/TREC/50_Results/Progress Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\50_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC73BEAE-0D0B-43DA-B54A-563246F3C364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2160569-855E-418B-B93C-06BFCE44D04D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
@@ -1620,7 +1620,7 @@
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2001,6 +2001,11 @@
     <xf numFmtId="0" fontId="38" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2334,7 +2339,7 @@
   <dimension ref="B2:XFD369"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="32" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11647,9 +11652,15 @@
       <c r="K31" s="208"/>
       <c r="L31" s="209"/>
       <c r="M31" s="210"/>
-      <c r="N31" s="202"/>
-      <c r="O31" s="211"/>
-      <c r="P31" s="204"/>
+      <c r="N31" s="230">
+        <v>0.8</v>
+      </c>
+      <c r="O31" s="232">
+        <v>0.7</v>
+      </c>
+      <c r="P31" s="231">
+        <v>0.7</v>
+      </c>
       <c r="Q31" s="179"/>
       <c r="R31" s="15"/>
       <c r="S31" s="15"/>
@@ -11688,9 +11699,15 @@
       <c r="K32" s="208"/>
       <c r="L32" s="209"/>
       <c r="M32" s="210"/>
-      <c r="N32" s="202"/>
-      <c r="O32" s="211"/>
-      <c r="P32" s="204"/>
+      <c r="N32" s="230">
+        <v>0.75</v>
+      </c>
+      <c r="O32" s="232">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="P32" s="231">
+        <v>0.625</v>
+      </c>
       <c r="Q32" s="179"/>
       <c r="R32" s="15"/>
       <c r="S32" s="15"/>
@@ -11731,9 +11748,15 @@
       <c r="K33" s="208"/>
       <c r="L33" s="209"/>
       <c r="M33" s="210"/>
-      <c r="N33" s="202"/>
-      <c r="O33" s="211"/>
-      <c r="P33" s="204"/>
+      <c r="N33" s="230">
+        <v>0.8</v>
+      </c>
+      <c r="O33" s="232">
+        <v>0.7</v>
+      </c>
+      <c r="P33" s="231">
+        <v>0.7</v>
+      </c>
       <c r="Q33" s="179"/>
       <c r="R33" s="15"/>
       <c r="S33" s="15"/>
@@ -11772,9 +11795,15 @@
       <c r="K34" s="208"/>
       <c r="L34" s="209"/>
       <c r="M34" s="210"/>
-      <c r="N34" s="202"/>
-      <c r="O34" s="211"/>
-      <c r="P34" s="204"/>
+      <c r="N34" s="230">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O34" s="232">
+        <v>2E-3</v>
+      </c>
+      <c r="P34" s="231">
+        <v>4.4000000000000003E-3</v>
+      </c>
       <c r="Q34" s="179"/>
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
@@ -11813,9 +11842,15 @@
       <c r="K35" s="208"/>
       <c r="L35" s="209"/>
       <c r="M35" s="210"/>
-      <c r="N35" s="202"/>
-      <c r="O35" s="211"/>
-      <c r="P35" s="204"/>
+      <c r="N35" s="230">
+        <v>0.75</v>
+      </c>
+      <c r="O35" s="232">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="P35" s="231">
+        <v>0.625</v>
+      </c>
       <c r="Q35" s="179"/>
       <c r="R35" s="15"/>
       <c r="S35" s="15"/>
@@ -11854,9 +11889,15 @@
       <c r="K36" s="208"/>
       <c r="L36" s="209"/>
       <c r="M36" s="210"/>
-      <c r="N36" s="202"/>
-      <c r="O36" s="211"/>
-      <c r="P36" s="204"/>
+      <c r="N36" s="230">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="O36" s="232">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P36" s="231">
+        <v>6.6E-3</v>
+      </c>
       <c r="Q36" s="179"/>
       <c r="R36" s="15"/>
       <c r="S36" s="15"/>

</xml_diff>

<commit_message>
Final LSTM Glove code and summary updated
</commit_message>
<xml_diff>
--- a/TREC/50_Results/Progress Summary.xlsx
+++ b/TREC/50_Results/Progress Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishaal\Documents\GitHub\TREC_Distributed_Machine_Learning\TREC\50_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2160569-855E-418B-B93C-06BFCE44D04D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49ECA11-8F19-45EB-82F8-85BD62AB7EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{4C32F7FF-54D9-41F1-8D11-CF21E2614B25}"/>
   </bookViews>
@@ -1620,7 +1620,7 @@
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="233">
+  <cellXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2006,6 +2006,11 @@
     <xf numFmtId="0" fontId="35" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2339,7 +2344,7 @@
   <dimension ref="B2:XFD369"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="32" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+      <selection activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11944,9 +11949,15 @@
       <c r="M37" s="228">
         <v>0.73</v>
       </c>
-      <c r="N37" s="202"/>
-      <c r="O37" s="211"/>
-      <c r="P37" s="204"/>
+      <c r="N37" s="233">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="O37" s="235">
+        <v>0.6</v>
+      </c>
+      <c r="P37" s="234">
+        <v>0.66669999999999996</v>
+      </c>
       <c r="Q37" s="179"/>
       <c r="R37" s="15"/>
       <c r="S37" s="15"/>
@@ -11991,9 +12002,15 @@
       <c r="M38" s="228">
         <v>0.67</v>
       </c>
-      <c r="N38" s="202"/>
-      <c r="O38" s="211"/>
-      <c r="P38" s="204"/>
+      <c r="N38" s="233">
+        <v>0.61109999999999998</v>
+      </c>
+      <c r="O38" s="235">
+        <v>0.44440000000000002</v>
+      </c>
+      <c r="P38" s="234">
+        <v>0.5</v>
+      </c>
       <c r="Q38" s="179"/>
       <c r="R38" s="15"/>
       <c r="S38" s="15"/>

</xml_diff>